<commit_message>
Results with analysis, just 3 mistakes in the 900/600 samples
</commit_message>
<xml_diff>
--- a/Results/Final Results/Samples/100Scen/Results_Sample100_01.xlsx
+++ b/Results/Final Results/Samples/100Scen/Results_Sample100_01.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\charl\OneDrive\Dokumente\6.Semester\Bachelor-Arbeit\bachelor-thesis\bachelor-thesis\Results\Final Results\Samples\100Scen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CBEA88B-628F-40E8-B56C-9514BA97D87B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9349D3A9-F81B-4D86-8467-53CDCC7EA629}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -161,9 +161,6 @@
     <t>Steprule</t>
   </si>
   <si>
-    <t>Nullhypothesis: (MeanGap)_LR &lt;= (MeanGap)_Naive</t>
-  </si>
-  <si>
     <t>unable to reject</t>
   </si>
   <si>
@@ -267,6 +264,9 @@
   </si>
   <si>
     <t>NOCH NICHT GEMACHT</t>
+  </si>
+  <si>
+    <t>Nullhypothesis: (MeanGap)_LR &gt; (MeanGap)_Naive</t>
   </si>
 </sst>
 </file>
@@ -679,7 +679,7 @@
   <dimension ref="A1:U121"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="U5" sqref="U5"/>
+      <selection activeCell="R6" sqref="R6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -755,7 +755,7 @@
         <v>16</v>
       </c>
       <c r="S1" t="s">
-        <v>17</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.35">
@@ -855,7 +855,7 @@
         <v>1</v>
       </c>
       <c r="S3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.35">
@@ -905,7 +905,7 @@
         <v>2</v>
       </c>
       <c r="S4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.35">
@@ -955,10 +955,10 @@
         <v>3</v>
       </c>
       <c r="S5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="U5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.35">
@@ -1008,7 +1008,7 @@
         <v>4</v>
       </c>
       <c r="S6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.35">
@@ -1058,7 +1058,7 @@
         <v>5</v>
       </c>
       <c r="S7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.35">
@@ -1111,7 +1111,7 @@
         <v>6</v>
       </c>
       <c r="S8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.35">
@@ -1249,10 +1249,10 @@
         <v>15</v>
       </c>
       <c r="R11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="S11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.35">
@@ -1346,10 +1346,10 @@
         <v>0.05</v>
       </c>
       <c r="R13" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="S13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.35">
@@ -1399,10 +1399,10 @@
         <v>274.54435999999998</v>
       </c>
       <c r="R14" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="S14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.35">
@@ -1449,10 +1449,10 @@
         <v>274.54435999999998</v>
       </c>
       <c r="R15" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="S15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.35">
@@ -1499,10 +1499,10 @@
         <v>274.54435999999998</v>
       </c>
       <c r="R16" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.35">
@@ -1549,10 +1549,10 @@
         <v>274.54435999999998</v>
       </c>
       <c r="R17" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="S17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.35">
@@ -1599,10 +1599,10 @@
         <v>274.54435999999998</v>
       </c>
       <c r="R18" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="S18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.35">
@@ -1649,10 +1649,10 @@
         <v>274.54435999999998</v>
       </c>
       <c r="R19" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.35">
@@ -1702,10 +1702,10 @@
         <v>267.64940000000001</v>
       </c>
       <c r="R20" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="S20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.35">
@@ -1752,10 +1752,10 @@
         <v>267.64940000000001</v>
       </c>
       <c r="R21" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="S21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.35">
@@ -1802,10 +1802,10 @@
         <v>267.64940000000001</v>
       </c>
       <c r="R22" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="S22" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.35">
@@ -1852,10 +1852,10 @@
         <v>267.64940000000001</v>
       </c>
       <c r="R23" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="S23" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.35">
@@ -1902,10 +1902,10 @@
         <v>267.64940000000001</v>
       </c>
       <c r="R24" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S24" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.35">
@@ -1952,10 +1952,10 @@
         <v>267.64940000000001</v>
       </c>
       <c r="R25" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="S25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.35">
@@ -2005,10 +2005,10 @@
         <v>268.45136000000002</v>
       </c>
       <c r="R26" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="S26" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.35">
@@ -2055,10 +2055,10 @@
         <v>268.45136000000002</v>
       </c>
       <c r="R27" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="S27" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.35">
@@ -2105,10 +2105,10 @@
         <v>268.45136000000002</v>
       </c>
       <c r="R28" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="S28" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.35">
@@ -2155,10 +2155,10 @@
         <v>268.45136000000002</v>
       </c>
       <c r="R29" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="S29" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.35">
@@ -2205,10 +2205,10 @@
         <v>268.45136000000002</v>
       </c>
       <c r="R30" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="S30" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.35">
@@ -2255,10 +2255,10 @@
         <v>268.45136000000002</v>
       </c>
       <c r="R31" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="S31" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.35">
@@ -2308,10 +2308,10 @@
         <v>269.93166000000002</v>
       </c>
       <c r="R32" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="S32" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.35">
@@ -2358,10 +2358,10 @@
         <v>269.93166000000002</v>
       </c>
       <c r="R33" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="S33" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.35">
@@ -2408,10 +2408,10 @@
         <v>269.93166000000002</v>
       </c>
       <c r="R34" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="S34" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.35">
@@ -2458,10 +2458,10 @@
         <v>269.93166000000002</v>
       </c>
       <c r="R35" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="S35" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.35">
@@ -2508,10 +2508,10 @@
         <v>269.93166000000002</v>
       </c>
       <c r="R36" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="S36" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.35">
@@ -2558,10 +2558,10 @@
         <v>269.93166000000002</v>
       </c>
       <c r="R37" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="S37" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.35">
@@ -2611,10 +2611,10 @@
         <v>275.64729999999997</v>
       </c>
       <c r="R38" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="S38" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.35">
@@ -2661,10 +2661,10 @@
         <v>275.64729999999997</v>
       </c>
       <c r="R39" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="S39" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.35">
@@ -2711,10 +2711,10 @@
         <v>275.64729999999997</v>
       </c>
       <c r="R40" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="S40" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.35">
@@ -2761,10 +2761,10 @@
         <v>275.64729999999997</v>
       </c>
       <c r="R41" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="S41" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.35">
@@ -2811,10 +2811,10 @@
         <v>275.64729999999997</v>
       </c>
       <c r="R42" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="S42" t="s">
         <v>50</v>
-      </c>
-      <c r="S42" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.35">

</xml_diff>